<commit_message>
- added lab test grades
</commit_message>
<xml_diff>
--- a/Students/30421/Lab30421.xlsx
+++ b/Students/30421/Lab30421.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="50">
   <si>
     <t>Nume si prenume</t>
   </si>
@@ -158,6 +158,12 @@
   </si>
   <si>
     <t>Final mark</t>
+  </si>
+  <si>
+    <t>fail</t>
+  </si>
+  <si>
+    <t>pass</t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1082,7 @@
   <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+      <selection activeCell="Q2" sqref="Q2:U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,18 +1245,16 @@
         <v>0.2</v>
       </c>
       <c r="R3" s="6">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="S3" s="6">
-        <v>5.5</v>
+        <v>4.3</v>
       </c>
       <c r="T3" s="6">
-        <f>IF((R3+S3)/2 + Q3 &gt; 10, 10, (R3+S3)/2 + Q3)</f>
-        <v>3.45</v>
-      </c>
-      <c r="U3" s="6" t="str">
-        <f>IF(AND(R3&gt;5, S3&gt;5), "pass", "fail")</f>
-        <v>fail</v>
+        <v>7.35</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1308,15 +1312,13 @@
         <v>6.5</v>
       </c>
       <c r="S4" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T4" s="5">
-        <f>IF((R4+S4)/2 + Q4 &gt; 10, 10, (R4+S4)/2 + Q4)</f>
-        <v>3.9</v>
-      </c>
-      <c r="U4" s="5" t="str">
-        <f t="shared" ref="U4:U25" si="1">IF(AND(R4&gt;5, S4&gt;5), "pass", "fail")</f>
-        <v>fail</v>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1377,12 +1379,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="T5" s="6">
-        <f t="shared" ref="T5:T25" si="2">IF((R5+S5)/2 + Q5 &gt; 10, 10, (R5+S5)/2 + Q5)</f>
         <v>9.6</v>
       </c>
-      <c r="U5" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U5" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1437,18 +1437,16 @@
         <v>0.3</v>
       </c>
       <c r="R6" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="S6" s="5">
-        <v>1</v>
+        <v>3.2</v>
       </c>
       <c r="T6" s="5">
-        <f t="shared" si="2"/>
-        <v>1.3</v>
-      </c>
-      <c r="U6" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>5.4</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1509,12 +1507,10 @@
         <v>7.6</v>
       </c>
       <c r="T7" s="6">
-        <f t="shared" si="2"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="U7" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U7" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1569,18 +1565,16 @@
         <v>0.1</v>
       </c>
       <c r="R8" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S8" s="5">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="T8" s="5">
-        <f t="shared" si="2"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="U8" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>3.5</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1635,18 +1629,16 @@
         <v>0.15</v>
       </c>
       <c r="R9" s="6">
-        <v>1</v>
+        <v>8.75</v>
       </c>
       <c r="S9" s="6">
-        <v>1</v>
+        <v>8.9</v>
       </c>
       <c r="T9" s="6">
-        <f t="shared" si="2"/>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="U9" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>8.9749999999999996</v>
+      </c>
+      <c r="U9" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1704,15 +1696,13 @@
         <v>6</v>
       </c>
       <c r="S10" s="5">
-        <v>2.8</v>
+        <v>3.1</v>
       </c>
       <c r="T10" s="5">
-        <f t="shared" si="2"/>
-        <v>4.53</v>
-      </c>
-      <c r="U10" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>4.68</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1767,18 +1757,16 @@
         <v>0.08</v>
       </c>
       <c r="R11" s="6">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="S11" s="6">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="T11" s="6">
-        <f t="shared" si="2"/>
-        <v>3.58</v>
-      </c>
-      <c r="U11" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>4.88</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1839,12 +1827,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="T12" s="5">
-        <f t="shared" si="2"/>
         <v>6.38</v>
       </c>
-      <c r="U12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+      <c r="U12" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1902,15 +1888,13 @@
         <v>10</v>
       </c>
       <c r="S13" s="6">
-        <v>4.3</v>
+        <v>7.1</v>
       </c>
       <c r="T13" s="6">
-        <f t="shared" si="2"/>
-        <v>7.33</v>
-      </c>
-      <c r="U13" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>8.73</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -1965,18 +1949,16 @@
         <v>0.18</v>
       </c>
       <c r="R14" s="5">
-        <v>1</v>
+        <v>9.25</v>
       </c>
       <c r="S14" s="5">
-        <v>4.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="T14" s="5">
-        <f t="shared" si="2"/>
-        <v>2.7800000000000002</v>
-      </c>
-      <c r="U14" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>9.4049999999999994</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2034,15 +2016,13 @@
         <v>9.5</v>
       </c>
       <c r="S15" s="6">
-        <v>3</v>
+        <v>7.9</v>
       </c>
       <c r="T15" s="6">
-        <f t="shared" si="2"/>
-        <v>6.44</v>
-      </c>
-      <c r="U15" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>8.89</v>
+      </c>
+      <c r="U15" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2103,12 +2083,10 @@
         <v>5.8</v>
       </c>
       <c r="T16" s="5">
-        <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="U16" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U16" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2169,12 +2147,10 @@
         <v>7.4</v>
       </c>
       <c r="T17" s="6">
-        <f t="shared" si="2"/>
         <v>8.6999999999999993</v>
       </c>
-      <c r="U17" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U17" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2231,12 +2207,10 @@
         <v>1</v>
       </c>
       <c r="T18" s="5">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U18" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+      <c r="U18" s="5" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2297,12 +2271,10 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="T19" s="6">
-        <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
-      <c r="U19" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U19" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2359,12 +2331,10 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="T20" s="5">
-        <f t="shared" si="2"/>
         <v>8.85</v>
       </c>
-      <c r="U20" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U20" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2425,12 +2395,10 @@
         <v>8.4</v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="U21" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U21" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2485,18 +2453,16 @@
         <v>0.12</v>
       </c>
       <c r="R22" s="5">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="S22" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="T22" s="5">
-        <f t="shared" si="2"/>
-        <v>2.62</v>
-      </c>
-      <c r="U22" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>6.37</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2549,12 +2515,10 @@
         <v>1</v>
       </c>
       <c r="T23" s="6">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="U23" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+      <c r="U23" s="6" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2609,18 +2573,16 @@
         <v>0.15</v>
       </c>
       <c r="R24" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="S24" s="5">
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="T24" s="5">
-        <f t="shared" si="2"/>
-        <v>2.9</v>
-      </c>
-      <c r="U24" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>fail</v>
+        <v>5.7</v>
+      </c>
+      <c r="U24" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -2681,12 +2643,10 @@
         <v>9.6</v>
       </c>
       <c r="T25" s="6">
-        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="U25" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>pass</v>
+      <c r="U25" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>